<commit_message>
MDT producten toegevoegd WIP
</commit_message>
<xml_diff>
--- a/MDT/DienstenCatalogus/Producten-RegistratieDocumentAfhandeling.xlsx
+++ b/MDT/DienstenCatalogus/Producten-RegistratieDocumentAfhandeling.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="198">
   <si>
     <t>PROD_CODE</t>
   </si>
@@ -576,18 +576,12 @@
     <t>Product</t>
   </si>
   <si>
-    <t>omschrijvingRda</t>
-  </si>
-  <si>
     <t>ProductRDA</t>
   </si>
   <si>
     <t>[ProductRDA]</t>
   </si>
   <si>
-    <t>rdwProd</t>
-  </si>
-  <si>
     <t>presentatieGroep</t>
   </si>
   <si>
@@ -600,7 +594,28 @@
     <t>ProcID</t>
   </si>
   <si>
-    <t>OmschrijvingProduct</t>
+    <t>organisatieOnd</t>
+  </si>
+  <si>
+    <t>OrganisatieOnderdeel</t>
+  </si>
+  <si>
+    <t>bron</t>
+  </si>
+  <si>
+    <t>Bron</t>
+  </si>
+  <si>
+    <t>RDA</t>
+  </si>
+  <si>
+    <t>ProductOmschrijving</t>
+  </si>
+  <si>
+    <t>omschrijving</t>
+  </si>
+  <si>
+    <t>rdwProduct</t>
   </si>
 </sst>
 </file>
@@ -750,7 +765,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -936,6 +951,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1097,10 +1118,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1446,10 +1468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J79"/>
+  <dimension ref="A1:K79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1464,9 +1486,10 @@
     <col min="8" max="8" width="17.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.77734375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1492,41 +1515,53 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C2" t="s">
+        <v>197</v>
+      </c>
+      <c r="E2" t="s">
+        <v>188</v>
+      </c>
+      <c r="H2" t="s">
+        <v>190</v>
+      </c>
+      <c r="I2" t="s">
         <v>186</v>
       </c>
-      <c r="B2" t="s">
+      <c r="K2" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>184</v>
       </c>
-      <c r="C2" t="s">
-        <v>187</v>
-      </c>
-      <c r="E2" t="s">
-        <v>190</v>
-      </c>
-      <c r="I2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>185</v>
-      </c>
       <c r="B3" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="C3" t="s">
         <v>183</v>
       </c>
       <c r="E3" t="s">
+        <v>189</v>
+      </c>
+      <c r="H3" t="s">
         <v>191</v>
       </c>
       <c r="I3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1559,8 +1594,11 @@
       <c r="J4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K4" s="3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1587,8 +1625,12 @@
       <c r="I5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K5" s="3" t="str">
+        <f>K4</f>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1603,7 +1645,7 @@
         <v>30440106</v>
       </c>
       <c r="E6" s="2" t="str">
-        <f t="shared" ref="C6:E12" si="3">IF(F6=0,"",IF(ISNUMBER(F6),TEXT(F6,"0"),F6))</f>
+        <f t="shared" ref="E6:E12" si="3">IF(F6=0,"",IF(ISNUMBER(F6),TEXT(F6,"0"),F6))</f>
         <v>2731</v>
       </c>
       <c r="F6">
@@ -1621,8 +1663,12 @@
       <c r="J6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K6" s="3" t="str">
+        <f t="shared" ref="K6:K69" si="4">K5</f>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1630,7 +1676,7 @@
         <v>20</v>
       </c>
       <c r="C7" s="2" t="str">
-        <f t="shared" ref="C7" si="4">IF(D7=0,"",IF(ISNUMBER(D7),TEXT(D7,"0"),D7))</f>
+        <f t="shared" ref="C7" si="5">IF(D7=0,"",IF(ISNUMBER(D7),TEXT(D7,"0"),D7))</f>
         <v/>
       </c>
       <c r="E7" s="2" t="str">
@@ -1649,8 +1695,12 @@
       <c r="I7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K7" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1658,7 +1708,7 @@
         <v>22</v>
       </c>
       <c r="C8" s="2" t="str">
-        <f t="shared" ref="C8" si="5">IF(D8=0,"",IF(ISNUMBER(D8),TEXT(D8,"0"),D8))</f>
+        <f t="shared" ref="C8" si="6">IF(D8=0,"",IF(ISNUMBER(D8),TEXT(D8,"0"),D8))</f>
         <v/>
       </c>
       <c r="E8" s="2" t="str">
@@ -1680,8 +1730,12 @@
       <c r="J8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K8" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -1689,7 +1743,7 @@
         <v>25</v>
       </c>
       <c r="C9" s="2" t="str">
-        <f t="shared" ref="C9" si="6">IF(D9=0,"",IF(ISNUMBER(D9),TEXT(D9,"0"),D9))</f>
+        <f t="shared" ref="C9" si="7">IF(D9=0,"",IF(ISNUMBER(D9),TEXT(D9,"0"),D9))</f>
         <v>30440107</v>
       </c>
       <c r="D9">
@@ -1714,8 +1768,12 @@
       <c r="J9">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K9" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1723,7 +1781,7 @@
         <v>27</v>
       </c>
       <c r="C10" s="2" t="str">
-        <f t="shared" ref="C10" si="7">IF(D10=0,"",IF(ISNUMBER(D10),TEXT(D10,"0"),D10))</f>
+        <f t="shared" ref="C10" si="8">IF(D10=0,"",IF(ISNUMBER(D10),TEXT(D10,"0"),D10))</f>
         <v/>
       </c>
       <c r="E10" s="2" t="str">
@@ -1745,8 +1803,12 @@
       <c r="J10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K10" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -1754,7 +1816,7 @@
         <v>30</v>
       </c>
       <c r="C11" s="2" t="str">
-        <f t="shared" ref="C11" si="8">IF(D11=0,"",IF(ISNUMBER(D11),TEXT(D11,"0"),D11))</f>
+        <f t="shared" ref="C11" si="9">IF(D11=0,"",IF(ISNUMBER(D11),TEXT(D11,"0"),D11))</f>
         <v/>
       </c>
       <c r="E11" s="2" t="str">
@@ -1773,8 +1835,12 @@
       <c r="I11" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K11" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -1782,7 +1848,7 @@
         <v>33</v>
       </c>
       <c r="C12" s="2" t="str">
-        <f t="shared" ref="C12" si="9">IF(D12=0,"",IF(ISNUMBER(D12),TEXT(D12,"0"),D12))</f>
+        <f t="shared" ref="C12" si="10">IF(D12=0,"",IF(ISNUMBER(D12),TEXT(D12,"0"),D12))</f>
         <v/>
       </c>
       <c r="E12" s="2" t="str">
@@ -1804,8 +1870,12 @@
       <c r="J12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K12" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -1813,11 +1883,11 @@
         <v>36</v>
       </c>
       <c r="C13" s="2" t="str">
-        <f t="shared" ref="C13" si="10">IF(D13=0,"",IF(ISNUMBER(D13),TEXT(D13,"0"),D13))</f>
+        <f t="shared" ref="C13" si="11">IF(D13=0,"",IF(ISNUMBER(D13),TEXT(D13,"0"),D13))</f>
         <v/>
       </c>
       <c r="E13" s="2" t="str">
-        <f t="shared" ref="C4:E67" si="11">IF(ISNUMBER(F13),TEXT(F13,"0"),F13)</f>
+        <f t="shared" ref="E13:E67" si="12">IF(ISNUMBER(F13),TEXT(F13,"0"),F13)</f>
         <v>2685</v>
       </c>
       <c r="F13">
@@ -1835,8 +1905,12 @@
       <c r="J13">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K13" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -1844,11 +1918,11 @@
         <v>39</v>
       </c>
       <c r="C14" s="2" t="str">
-        <f t="shared" ref="C14" si="12">IF(D14=0,"",IF(ISNUMBER(D14),TEXT(D14,"0"),D14))</f>
+        <f t="shared" ref="C14" si="13">IF(D14=0,"",IF(ISNUMBER(D14),TEXT(D14,"0"),D14))</f>
         <v/>
       </c>
       <c r="E14" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2105</v>
       </c>
       <c r="F14">
@@ -1860,8 +1934,12 @@
       <c r="H14" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K14" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>40</v>
       </c>
@@ -1869,11 +1947,11 @@
         <v>41</v>
       </c>
       <c r="C15" s="2" t="str">
-        <f t="shared" ref="C15" si="13">IF(D15=0,"",IF(ISNUMBER(D15),TEXT(D15,"0"),D15))</f>
+        <f t="shared" ref="C15" si="14">IF(D15=0,"",IF(ISNUMBER(D15),TEXT(D15,"0"),D15))</f>
         <v/>
       </c>
       <c r="E15" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2471</v>
       </c>
       <c r="F15">
@@ -1891,8 +1969,12 @@
       <c r="J15">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K15" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>43</v>
       </c>
@@ -1900,11 +1982,11 @@
         <v>44</v>
       </c>
       <c r="C16" s="2" t="str">
-        <f t="shared" ref="C16" si="14">IF(D16=0,"",IF(ISNUMBER(D16),TEXT(D16,"0"),D16))</f>
+        <f t="shared" ref="C16" si="15">IF(D16=0,"",IF(ISNUMBER(D16),TEXT(D16,"0"),D16))</f>
         <v/>
       </c>
       <c r="E16" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2472</v>
       </c>
       <c r="F16">
@@ -1922,8 +2004,12 @@
       <c r="J16">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K16" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>45</v>
       </c>
@@ -1931,11 +2017,11 @@
         <v>46</v>
       </c>
       <c r="C17" s="2" t="str">
-        <f t="shared" ref="C17" si="15">IF(D17=0,"",IF(ISNUMBER(D17),TEXT(D17,"0"),D17))</f>
+        <f t="shared" ref="C17" si="16">IF(D17=0,"",IF(ISNUMBER(D17),TEXT(D17,"0"),D17))</f>
         <v/>
       </c>
       <c r="E17" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2592</v>
       </c>
       <c r="F17">
@@ -1953,8 +2039,12 @@
       <c r="J17">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K17" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>47</v>
       </c>
@@ -1962,11 +2052,11 @@
         <v>48</v>
       </c>
       <c r="C18" s="2" t="str">
-        <f t="shared" ref="C18" si="16">IF(D18=0,"",IF(ISNUMBER(D18),TEXT(D18,"0"),D18))</f>
+        <f t="shared" ref="C18" si="17">IF(D18=0,"",IF(ISNUMBER(D18),TEXT(D18,"0"),D18))</f>
         <v/>
       </c>
       <c r="E18" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2995</v>
       </c>
       <c r="F18">
@@ -1984,8 +2074,12 @@
       <c r="J18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K18" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>50</v>
       </c>
@@ -1993,11 +2087,11 @@
         <v>51</v>
       </c>
       <c r="C19" s="2" t="str">
-        <f t="shared" ref="C19" si="17">IF(D19=0,"",IF(ISNUMBER(D19),TEXT(D19,"0"),D19))</f>
+        <f t="shared" ref="C19" si="18">IF(D19=0,"",IF(ISNUMBER(D19),TEXT(D19,"0"),D19))</f>
         <v/>
       </c>
       <c r="E19" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2360</v>
       </c>
       <c r="F19">
@@ -2015,8 +2109,12 @@
       <c r="J19">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K19" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>52</v>
       </c>
@@ -2024,11 +2122,11 @@
         <v>53</v>
       </c>
       <c r="C20" s="2" t="str">
-        <f t="shared" ref="C20" si="18">IF(D20=0,"",IF(ISNUMBER(D20),TEXT(D20,"0"),D20))</f>
+        <f t="shared" ref="C20" si="19">IF(D20=0,"",IF(ISNUMBER(D20),TEXT(D20,"0"),D20))</f>
         <v/>
       </c>
       <c r="E20" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2363</v>
       </c>
       <c r="F20">
@@ -2046,8 +2144,12 @@
       <c r="J20">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K20" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>54</v>
       </c>
@@ -2055,11 +2157,11 @@
         <v>55</v>
       </c>
       <c r="C21" s="2" t="str">
-        <f t="shared" ref="C21" si="19">IF(D21=0,"",IF(ISNUMBER(D21),TEXT(D21,"0"),D21))</f>
+        <f t="shared" ref="C21" si="20">IF(D21=0,"",IF(ISNUMBER(D21),TEXT(D21,"0"),D21))</f>
         <v/>
       </c>
       <c r="E21" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2046</v>
       </c>
       <c r="F21">
@@ -2077,8 +2179,12 @@
       <c r="J21">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K21" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>57</v>
       </c>
@@ -2086,11 +2192,11 @@
         <v>58</v>
       </c>
       <c r="C22" s="2" t="str">
-        <f t="shared" ref="C22" si="20">IF(D22=0,"",IF(ISNUMBER(D22),TEXT(D22,"0"),D22))</f>
+        <f t="shared" ref="C22" si="21">IF(D22=0,"",IF(ISNUMBER(D22),TEXT(D22,"0"),D22))</f>
         <v/>
       </c>
       <c r="E22" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2180</v>
       </c>
       <c r="F22">
@@ -2108,8 +2214,12 @@
       <c r="J22">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K22" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>59</v>
       </c>
@@ -2117,14 +2227,14 @@
         <v>60</v>
       </c>
       <c r="C23" s="2" t="str">
-        <f t="shared" ref="C23" si="21">IF(D23=0,"",IF(ISNUMBER(D23),TEXT(D23,"0"),D23))</f>
+        <f t="shared" ref="C23" si="22">IF(D23=0,"",IF(ISNUMBER(D23),TEXT(D23,"0"),D23))</f>
         <v>30130301</v>
       </c>
       <c r="D23">
         <v>30130301</v>
       </c>
       <c r="E23" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2043</v>
       </c>
       <c r="F23">
@@ -2139,8 +2249,12 @@
       <c r="I23" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K23" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>61</v>
       </c>
@@ -2148,11 +2262,11 @@
         <v>62</v>
       </c>
       <c r="C24" s="2" t="str">
-        <f t="shared" ref="C24" si="22">IF(D24=0,"",IF(ISNUMBER(D24),TEXT(D24,"0"),D24))</f>
+        <f t="shared" ref="C24" si="23">IF(D24=0,"",IF(ISNUMBER(D24),TEXT(D24,"0"),D24))</f>
         <v/>
       </c>
       <c r="E24" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2045</v>
       </c>
       <c r="F24">
@@ -2170,8 +2284,12 @@
       <c r="J24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K24" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>63</v>
       </c>
@@ -2179,14 +2297,14 @@
         <v>64</v>
       </c>
       <c r="C25" s="2" t="str">
-        <f t="shared" ref="C25" si="23">IF(D25=0,"",IF(ISNUMBER(D25),TEXT(D25,"0"),D25))</f>
+        <f t="shared" ref="C25" si="24">IF(D25=0,"",IF(ISNUMBER(D25),TEXT(D25,"0"),D25))</f>
         <v>30130301</v>
       </c>
       <c r="D25">
         <v>30130301</v>
       </c>
       <c r="E25" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2620</v>
       </c>
       <c r="F25">
@@ -2204,8 +2322,12 @@
       <c r="J25">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K25" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>65</v>
       </c>
@@ -2213,14 +2335,14 @@
         <v>66</v>
       </c>
       <c r="C26" s="2" t="str">
-        <f t="shared" ref="C26" si="24">IF(D26=0,"",IF(ISNUMBER(D26),TEXT(D26,"0"),D26))</f>
+        <f t="shared" ref="C26" si="25">IF(D26=0,"",IF(ISNUMBER(D26),TEXT(D26,"0"),D26))</f>
         <v>30130301</v>
       </c>
       <c r="D26">
         <v>30130301</v>
       </c>
       <c r="E26" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2181</v>
       </c>
       <c r="F26">
@@ -2238,8 +2360,12 @@
       <c r="J26">
         <v>4</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K26" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>67</v>
       </c>
@@ -2247,11 +2373,11 @@
         <v>68</v>
       </c>
       <c r="C27" s="2" t="str">
-        <f t="shared" ref="C27" si="25">IF(D27=0,"",IF(ISNUMBER(D27),TEXT(D27,"0"),D27))</f>
+        <f t="shared" ref="C27" si="26">IF(D27=0,"",IF(ISNUMBER(D27),TEXT(D27,"0"),D27))</f>
         <v/>
       </c>
       <c r="E27" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1944</v>
       </c>
       <c r="F27">
@@ -2266,8 +2392,12 @@
       <c r="I27" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K27" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>70</v>
       </c>
@@ -2275,11 +2405,11 @@
         <v>71</v>
       </c>
       <c r="C28" s="2" t="str">
-        <f t="shared" ref="C28" si="26">IF(D28=0,"",IF(ISNUMBER(D28),TEXT(D28,"0"),D28))</f>
+        <f t="shared" ref="C28" si="27">IF(D28=0,"",IF(ISNUMBER(D28),TEXT(D28,"0"),D28))</f>
         <v/>
       </c>
       <c r="E28" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2734</v>
       </c>
       <c r="F28">
@@ -2297,8 +2427,12 @@
       <c r="J28">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K28" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>72</v>
       </c>
@@ -2306,11 +2440,11 @@
         <v>73</v>
       </c>
       <c r="C29" s="2" t="str">
-        <f t="shared" ref="C29" si="27">IF(D29=0,"",IF(ISNUMBER(D29),TEXT(D29,"0"),D29))</f>
+        <f t="shared" ref="C29" si="28">IF(D29=0,"",IF(ISNUMBER(D29),TEXT(D29,"0"),D29))</f>
         <v/>
       </c>
       <c r="E29" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1945</v>
       </c>
       <c r="F29">
@@ -2328,8 +2462,12 @@
       <c r="J29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K29" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>74</v>
       </c>
@@ -2337,11 +2475,11 @@
         <v>75</v>
       </c>
       <c r="C30" s="2" t="str">
-        <f t="shared" ref="C30" si="28">IF(D30=0,"",IF(ISNUMBER(D30),TEXT(D30,"0"),D30))</f>
+        <f t="shared" ref="C30" si="29">IF(D30=0,"",IF(ISNUMBER(D30),TEXT(D30,"0"),D30))</f>
         <v/>
       </c>
       <c r="E30" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2325</v>
       </c>
       <c r="F30">
@@ -2359,8 +2497,12 @@
       <c r="J30">
         <v>4</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K30" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>76</v>
       </c>
@@ -2368,11 +2510,11 @@
         <v>77</v>
       </c>
       <c r="C31" s="2" t="str">
-        <f t="shared" ref="C31" si="29">IF(D31=0,"",IF(ISNUMBER(D31),TEXT(D31,"0"),D31))</f>
+        <f t="shared" ref="C31" si="30">IF(D31=0,"",IF(ISNUMBER(D31),TEXT(D31,"0"),D31))</f>
         <v/>
       </c>
       <c r="E31" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2327</v>
       </c>
       <c r="F31">
@@ -2390,8 +2532,12 @@
       <c r="J31">
         <v>5</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K31" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>78</v>
       </c>
@@ -2399,11 +2545,11 @@
         <v>79</v>
       </c>
       <c r="C32" s="2" t="str">
-        <f t="shared" ref="C32" si="30">IF(D32=0,"",IF(ISNUMBER(D32),TEXT(D32,"0"),D32))</f>
+        <f t="shared" ref="C32" si="31">IF(D32=0,"",IF(ISNUMBER(D32),TEXT(D32,"0"),D32))</f>
         <v/>
       </c>
       <c r="E32" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1807</v>
       </c>
       <c r="F32">
@@ -2418,8 +2564,12 @@
       <c r="I32" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K32" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>80</v>
       </c>
@@ -2427,11 +2577,11 @@
         <v>81</v>
       </c>
       <c r="C33" s="2" t="str">
-        <f t="shared" ref="C33" si="31">IF(D33=0,"",IF(ISNUMBER(D33),TEXT(D33,"0"),D33))</f>
+        <f t="shared" ref="C33" si="32">IF(D33=0,"",IF(ISNUMBER(D33),TEXT(D33,"0"),D33))</f>
         <v/>
       </c>
       <c r="E33" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1956</v>
       </c>
       <c r="F33">
@@ -2449,8 +2599,12 @@
       <c r="J33">
         <v>4</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K33" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>82</v>
       </c>
@@ -2458,11 +2612,11 @@
         <v>83</v>
       </c>
       <c r="C34" s="2" t="str">
-        <f t="shared" ref="C34" si="32">IF(D34=0,"",IF(ISNUMBER(D34),TEXT(D34,"0"),D34))</f>
+        <f t="shared" ref="C34" si="33">IF(D34=0,"",IF(ISNUMBER(D34),TEXT(D34,"0"),D34))</f>
         <v/>
       </c>
       <c r="E34" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1955</v>
       </c>
       <c r="F34">
@@ -2480,8 +2634,12 @@
       <c r="J34">
         <v>3</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K34" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>84</v>
       </c>
@@ -2489,11 +2647,11 @@
         <v>85</v>
       </c>
       <c r="C35" s="2" t="str">
-        <f t="shared" ref="C35" si="33">IF(D35=0,"",IF(ISNUMBER(D35),TEXT(D35,"0"),D35))</f>
+        <f t="shared" ref="C35" si="34">IF(D35=0,"",IF(ISNUMBER(D35),TEXT(D35,"0"),D35))</f>
         <v/>
       </c>
       <c r="E35" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1954</v>
       </c>
       <c r="F35">
@@ -2511,8 +2669,12 @@
       <c r="J35">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K35" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>86</v>
       </c>
@@ -2520,11 +2682,11 @@
         <v>87</v>
       </c>
       <c r="C36" s="2" t="str">
-        <f t="shared" ref="C36" si="34">IF(D36=0,"",IF(ISNUMBER(D36),TEXT(D36,"0"),D36))</f>
+        <f t="shared" ref="C36" si="35">IF(D36=0,"",IF(ISNUMBER(D36),TEXT(D36,"0"),D36))</f>
         <v/>
       </c>
       <c r="E36" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1953</v>
       </c>
       <c r="F36">
@@ -2542,8 +2704,12 @@
       <c r="J36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K36" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>88</v>
       </c>
@@ -2551,14 +2717,14 @@
         <v>89</v>
       </c>
       <c r="C37" s="2" t="str">
-        <f t="shared" ref="C37" si="35">IF(D37=0,"",IF(ISNUMBER(D37),TEXT(D37,"0"),D37))</f>
+        <f t="shared" ref="C37" si="36">IF(D37=0,"",IF(ISNUMBER(D37),TEXT(D37,"0"),D37))</f>
         <v>30232101</v>
       </c>
       <c r="D37">
         <v>30232101</v>
       </c>
       <c r="E37" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1961</v>
       </c>
       <c r="F37">
@@ -2573,8 +2739,12 @@
       <c r="I37" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K37" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>91</v>
       </c>
@@ -2582,11 +2752,11 @@
         <v>92</v>
       </c>
       <c r="C38" s="2" t="str">
-        <f t="shared" ref="C38" si="36">IF(D38=0,"",IF(ISNUMBER(D38),TEXT(D38,"0"),D38))</f>
+        <f t="shared" ref="C38" si="37">IF(D38=0,"",IF(ISNUMBER(D38),TEXT(D38,"0"),D38))</f>
         <v/>
       </c>
       <c r="E38" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2980</v>
       </c>
       <c r="F38">
@@ -2604,8 +2774,12 @@
       <c r="J38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K38" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>94</v>
       </c>
@@ -2613,11 +2787,11 @@
         <v>95</v>
       </c>
       <c r="C39" s="2" t="str">
-        <f t="shared" ref="C39" si="37">IF(D39=0,"",IF(ISNUMBER(D39),TEXT(D39,"0"),D39))</f>
+        <f t="shared" ref="C39" si="38">IF(D39=0,"",IF(ISNUMBER(D39),TEXT(D39,"0"),D39))</f>
         <v/>
       </c>
       <c r="E39" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2735</v>
       </c>
       <c r="F39">
@@ -2635,8 +2809,12 @@
       <c r="J39">
         <v>4</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K39" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>96</v>
       </c>
@@ -2644,11 +2822,11 @@
         <v>97</v>
       </c>
       <c r="C40" s="2" t="str">
-        <f t="shared" ref="C40" si="38">IF(D40=0,"",IF(ISNUMBER(D40),TEXT(D40,"0"),D40))</f>
+        <f t="shared" ref="C40" si="39">IF(D40=0,"",IF(ISNUMBER(D40),TEXT(D40,"0"),D40))</f>
         <v/>
       </c>
       <c r="E40" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2377</v>
       </c>
       <c r="F40">
@@ -2663,8 +2841,12 @@
       <c r="I40" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K40" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>99</v>
       </c>
@@ -2672,11 +2854,11 @@
         <v>100</v>
       </c>
       <c r="C41" s="2" t="str">
-        <f t="shared" ref="C41" si="39">IF(D41=0,"",IF(ISNUMBER(D41),TEXT(D41,"0"),D41))</f>
+        <f t="shared" ref="C41" si="40">IF(D41=0,"",IF(ISNUMBER(D41),TEXT(D41,"0"),D41))</f>
         <v/>
       </c>
       <c r="E41" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2358</v>
       </c>
       <c r="F41">
@@ -2694,8 +2876,12 @@
       <c r="J41">
         <v>4</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K41" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>101</v>
       </c>
@@ -2703,11 +2889,11 @@
         <v>102</v>
       </c>
       <c r="C42" s="2" t="str">
-        <f t="shared" ref="C42" si="40">IF(D42=0,"",IF(ISNUMBER(D42),TEXT(D42,"0"),D42))</f>
+        <f t="shared" ref="C42" si="41">IF(D42=0,"",IF(ISNUMBER(D42),TEXT(D42,"0"),D42))</f>
         <v/>
       </c>
       <c r="E42" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1942</v>
       </c>
       <c r="F42">
@@ -2722,8 +2908,12 @@
       <c r="I42" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K42" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>104</v>
       </c>
@@ -2731,11 +2921,11 @@
         <v>105</v>
       </c>
       <c r="C43" s="2" t="str">
-        <f t="shared" ref="C43" si="41">IF(D43=0,"",IF(ISNUMBER(D43),TEXT(D43,"0"),D43))</f>
+        <f t="shared" ref="C43" si="42">IF(D43=0,"",IF(ISNUMBER(D43),TEXT(D43,"0"),D43))</f>
         <v/>
       </c>
       <c r="E43" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2013</v>
       </c>
       <c r="F43">
@@ -2750,8 +2940,12 @@
       <c r="I43" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K43" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>107</v>
       </c>
@@ -2759,11 +2953,11 @@
         <v>108</v>
       </c>
       <c r="C44" s="2" t="str">
-        <f t="shared" ref="C44" si="42">IF(D44=0,"",IF(ISNUMBER(D44),TEXT(D44,"0"),D44))</f>
+        <f t="shared" ref="C44" si="43">IF(D44=0,"",IF(ISNUMBER(D44),TEXT(D44,"0"),D44))</f>
         <v/>
       </c>
       <c r="E44" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2110</v>
       </c>
       <c r="F44">
@@ -2778,8 +2972,12 @@
       <c r="I44" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K44" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>109</v>
       </c>
@@ -2787,11 +2985,11 @@
         <v>110</v>
       </c>
       <c r="C45" s="2" t="str">
-        <f t="shared" ref="C45" si="43">IF(D45=0,"",IF(ISNUMBER(D45),TEXT(D45,"0"),D45))</f>
+        <f t="shared" ref="C45" si="44">IF(D45=0,"",IF(ISNUMBER(D45),TEXT(D45,"0"),D45))</f>
         <v/>
       </c>
       <c r="E45" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2468</v>
       </c>
       <c r="F45">
@@ -2809,8 +3007,12 @@
       <c r="J45">
         <v>4</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K45" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>111</v>
       </c>
@@ -2818,11 +3020,11 @@
         <v>112</v>
       </c>
       <c r="C46" s="2" t="str">
-        <f t="shared" ref="C46" si="44">IF(D46=0,"",IF(ISNUMBER(D46),TEXT(D46,"0"),D46))</f>
+        <f t="shared" ref="C46" si="45">IF(D46=0,"",IF(ISNUMBER(D46),TEXT(D46,"0"),D46))</f>
         <v/>
       </c>
       <c r="E46" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2106</v>
       </c>
       <c r="F46">
@@ -2834,8 +3036,12 @@
       <c r="H46" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K46" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>113</v>
       </c>
@@ -2843,11 +3049,11 @@
         <v>114</v>
       </c>
       <c r="C47" s="2" t="str">
-        <f t="shared" ref="C47" si="45">IF(D47=0,"",IF(ISNUMBER(D47),TEXT(D47,"0"),D47))</f>
+        <f t="shared" ref="C47" si="46">IF(D47=0,"",IF(ISNUMBER(D47),TEXT(D47,"0"),D47))</f>
         <v/>
       </c>
       <c r="E47" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2466</v>
       </c>
       <c r="F47">
@@ -2862,8 +3068,12 @@
       <c r="I47" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K47" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>115</v>
       </c>
@@ -2871,11 +3081,11 @@
         <v>116</v>
       </c>
       <c r="C48" s="2" t="str">
-        <f t="shared" ref="C48" si="46">IF(D48=0,"",IF(ISNUMBER(D48),TEXT(D48,"0"),D48))</f>
+        <f t="shared" ref="C48" si="47">IF(D48=0,"",IF(ISNUMBER(D48),TEXT(D48,"0"),D48))</f>
         <v/>
       </c>
       <c r="E48" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2058</v>
       </c>
       <c r="F48">
@@ -2890,8 +3100,12 @@
       <c r="I48" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K48" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>118</v>
       </c>
@@ -2899,11 +3113,11 @@
         <v>119</v>
       </c>
       <c r="C49" s="2" t="str">
-        <f t="shared" ref="C49" si="47">IF(D49=0,"",IF(ISNUMBER(D49),TEXT(D49,"0"),D49))</f>
+        <f t="shared" ref="C49" si="48">IF(D49=0,"",IF(ISNUMBER(D49),TEXT(D49,"0"),D49))</f>
         <v/>
       </c>
       <c r="E49" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2059</v>
       </c>
       <c r="F49">
@@ -2921,8 +3135,12 @@
       <c r="J49">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K49" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>120</v>
       </c>
@@ -2930,11 +3148,11 @@
         <v>121</v>
       </c>
       <c r="C50" s="2" t="str">
-        <f t="shared" ref="C50" si="48">IF(D50=0,"",IF(ISNUMBER(D50),TEXT(D50,"0"),D50))</f>
+        <f t="shared" ref="C50" si="49">IF(D50=0,"",IF(ISNUMBER(D50),TEXT(D50,"0"),D50))</f>
         <v/>
       </c>
       <c r="E50" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2324</v>
       </c>
       <c r="F50">
@@ -2949,8 +3167,12 @@
       <c r="I50" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K50" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>122</v>
       </c>
@@ -2958,11 +3180,11 @@
         <v>123</v>
       </c>
       <c r="C51" s="2" t="str">
-        <f t="shared" ref="C51" si="49">IF(D51=0,"",IF(ISNUMBER(D51),TEXT(D51,"0"),D51))</f>
+        <f t="shared" ref="C51" si="50">IF(D51=0,"",IF(ISNUMBER(D51),TEXT(D51,"0"),D51))</f>
         <v/>
       </c>
       <c r="E51" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2324</v>
       </c>
       <c r="F51">
@@ -2974,8 +3196,12 @@
       <c r="H51" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K51" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>124</v>
       </c>
@@ -2983,11 +3209,11 @@
         <v>125</v>
       </c>
       <c r="C52" s="2" t="str">
-        <f t="shared" ref="C52" si="50">IF(D52=0,"",IF(ISNUMBER(D52),TEXT(D52,"0"),D52))</f>
+        <f t="shared" ref="C52" si="51">IF(D52=0,"",IF(ISNUMBER(D52),TEXT(D52,"0"),D52))</f>
         <v/>
       </c>
       <c r="E52" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2473</v>
       </c>
       <c r="F52">
@@ -3002,8 +3228,12 @@
       <c r="I52" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K52" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>126</v>
       </c>
@@ -3011,11 +3241,11 @@
         <v>127</v>
       </c>
       <c r="C53" s="2" t="str">
-        <f t="shared" ref="C53" si="51">IF(D53=0,"",IF(ISNUMBER(D53),TEXT(D53,"0"),D53))</f>
+        <f t="shared" ref="C53" si="52">IF(D53=0,"",IF(ISNUMBER(D53),TEXT(D53,"0"),D53))</f>
         <v/>
       </c>
       <c r="E53" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2474</v>
       </c>
       <c r="F53">
@@ -3033,8 +3263,12 @@
       <c r="J53">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K53" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>128</v>
       </c>
@@ -3042,11 +3276,11 @@
         <v>129</v>
       </c>
       <c r="C54" s="2" t="str">
-        <f t="shared" ref="C54" si="52">IF(D54=0,"",IF(ISNUMBER(D54),TEXT(D54,"0"),D54))</f>
+        <f t="shared" ref="C54" si="53">IF(D54=0,"",IF(ISNUMBER(D54),TEXT(D54,"0"),D54))</f>
         <v/>
       </c>
       <c r="E54" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2063</v>
       </c>
       <c r="F54">
@@ -3058,8 +3292,12 @@
       <c r="H54" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K54" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>130</v>
       </c>
@@ -3067,11 +3305,11 @@
         <v>131</v>
       </c>
       <c r="C55" s="2" t="str">
-        <f t="shared" ref="C55" si="53">IF(D55=0,"",IF(ISNUMBER(D55),TEXT(D55,"0"),D55))</f>
+        <f t="shared" ref="C55" si="54">IF(D55=0,"",IF(ISNUMBER(D55),TEXT(D55,"0"),D55))</f>
         <v/>
       </c>
       <c r="E55" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>3016</v>
       </c>
       <c r="F55">
@@ -3089,8 +3327,12 @@
       <c r="J55">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K55" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>132</v>
       </c>
@@ -3098,14 +3340,14 @@
         <v>133</v>
       </c>
       <c r="C56" s="2" t="str">
-        <f t="shared" ref="C56" si="54">IF(D56=0,"",IF(ISNUMBER(D56),TEXT(D56,"0"),D56))</f>
+        <f t="shared" ref="C56" si="55">IF(D56=0,"",IF(ISNUMBER(D56),TEXT(D56,"0"),D56))</f>
         <v>30232101</v>
       </c>
       <c r="D56">
         <v>30232101</v>
       </c>
       <c r="E56" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1959</v>
       </c>
       <c r="F56">
@@ -3123,8 +3365,12 @@
       <c r="J56">
         <v>2</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K56" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>134</v>
       </c>
@@ -3132,11 +3378,11 @@
         <v>135</v>
       </c>
       <c r="C57" s="2" t="str">
-        <f t="shared" ref="C57" si="55">IF(D57=0,"",IF(ISNUMBER(D57),TEXT(D57,"0"),D57))</f>
+        <f t="shared" ref="C57" si="56">IF(D57=0,"",IF(ISNUMBER(D57),TEXT(D57,"0"),D57))</f>
         <v/>
       </c>
       <c r="E57" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1943</v>
       </c>
       <c r="F57">
@@ -3154,8 +3400,12 @@
       <c r="J57">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K57" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>136</v>
       </c>
@@ -3163,11 +3413,11 @@
         <v>137</v>
       </c>
       <c r="C58" s="2" t="str">
-        <f t="shared" ref="C58" si="56">IF(D58=0,"",IF(ISNUMBER(D58),TEXT(D58,"0"),D58))</f>
+        <f t="shared" ref="C58" si="57">IF(D58=0,"",IF(ISNUMBER(D58),TEXT(D58,"0"),D58))</f>
         <v/>
       </c>
       <c r="E58" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2467</v>
       </c>
       <c r="F58">
@@ -3185,8 +3435,12 @@
       <c r="J58">
         <v>8</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K58" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>138</v>
       </c>
@@ -3194,11 +3448,11 @@
         <v>139</v>
       </c>
       <c r="C59" s="2" t="str">
-        <f t="shared" ref="C59" si="57">IF(D59=0,"",IF(ISNUMBER(D59),TEXT(D59,"0"),D59))</f>
+        <f t="shared" ref="C59" si="58">IF(D59=0,"",IF(ISNUMBER(D59),TEXT(D59,"0"),D59))</f>
         <v/>
       </c>
       <c r="E59" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2484</v>
       </c>
       <c r="F59">
@@ -3216,8 +3470,12 @@
       <c r="J59">
         <v>2</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K59" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>140</v>
       </c>
@@ -3225,11 +3483,11 @@
         <v>141</v>
       </c>
       <c r="C60" s="2" t="str">
-        <f t="shared" ref="C60" si="58">IF(D60=0,"",IF(ISNUMBER(D60),TEXT(D60,"0"),D60))</f>
+        <f t="shared" ref="C60" si="59">IF(D60=0,"",IF(ISNUMBER(D60),TEXT(D60,"0"),D60))</f>
         <v/>
       </c>
       <c r="E60" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2485</v>
       </c>
       <c r="F60">
@@ -3247,8 +3505,12 @@
       <c r="J60">
         <v>3</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K60" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>142</v>
       </c>
@@ -3256,11 +3518,11 @@
         <v>143</v>
       </c>
       <c r="C61" s="2" t="str">
-        <f t="shared" ref="C61" si="59">IF(D61=0,"",IF(ISNUMBER(D61),TEXT(D61,"0"),D61))</f>
+        <f t="shared" ref="C61" si="60">IF(D61=0,"",IF(ISNUMBER(D61),TEXT(D61,"0"),D61))</f>
         <v/>
       </c>
       <c r="E61" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2096</v>
       </c>
       <c r="F61">
@@ -3272,8 +3534,12 @@
       <c r="H61" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K61" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>144</v>
       </c>
@@ -3281,11 +3547,11 @@
         <v>145</v>
       </c>
       <c r="C62" s="2" t="str">
-        <f t="shared" ref="C62" si="60">IF(D62=0,"",IF(ISNUMBER(D62),TEXT(D62,"0"),D62))</f>
+        <f t="shared" ref="C62" si="61">IF(D62=0,"",IF(ISNUMBER(D62),TEXT(D62,"0"),D62))</f>
         <v/>
       </c>
       <c r="E62" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2469</v>
       </c>
       <c r="F62">
@@ -3303,8 +3569,12 @@
       <c r="J62">
         <v>6</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K62" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>146</v>
       </c>
@@ -3312,11 +3582,11 @@
         <v>147</v>
       </c>
       <c r="C63" s="2" t="str">
-        <f t="shared" ref="C63" si="61">IF(D63=0,"",IF(ISNUMBER(D63),TEXT(D63,"0"),D63))</f>
+        <f t="shared" ref="C63" si="62">IF(D63=0,"",IF(ISNUMBER(D63),TEXT(D63,"0"),D63))</f>
         <v/>
       </c>
       <c r="E63" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2589</v>
       </c>
       <c r="F63">
@@ -3334,8 +3604,12 @@
       <c r="J63">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K63" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>148</v>
       </c>
@@ -3343,11 +3617,11 @@
         <v>149</v>
       </c>
       <c r="C64" s="2" t="str">
-        <f t="shared" ref="C64" si="62">IF(D64=0,"",IF(ISNUMBER(D64),TEXT(D64,"0"),D64))</f>
+        <f t="shared" ref="C64" si="63">IF(D64=0,"",IF(ISNUMBER(D64),TEXT(D64,"0"),D64))</f>
         <v/>
       </c>
       <c r="E64" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2795</v>
       </c>
       <c r="F64">
@@ -3365,8 +3639,12 @@
       <c r="J64">
         <v>7</v>
       </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K64" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>150</v>
       </c>
@@ -3374,11 +3652,11 @@
         <v>151</v>
       </c>
       <c r="C65" s="2" t="str">
-        <f t="shared" ref="C65" si="63">IF(D65=0,"",IF(ISNUMBER(D65),TEXT(D65,"0"),D65))</f>
+        <f t="shared" ref="C65" si="64">IF(D65=0,"",IF(ISNUMBER(D65),TEXT(D65,"0"),D65))</f>
         <v/>
       </c>
       <c r="E65" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1946</v>
       </c>
       <c r="F65">
@@ -3393,8 +3671,12 @@
       <c r="I65" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K65" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>153</v>
       </c>
@@ -3402,14 +3684,14 @@
         <v>154</v>
       </c>
       <c r="C66" s="2" t="str">
-        <f t="shared" ref="C66" si="64">IF(D66=0,"",IF(ISNUMBER(D66),TEXT(D66,"0"),D66))</f>
+        <f t="shared" ref="C66" si="65">IF(D66=0,"",IF(ISNUMBER(D66),TEXT(D66,"0"),D66))</f>
         <v>30232101</v>
       </c>
       <c r="D66">
         <v>30232101</v>
       </c>
       <c r="E66" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1957</v>
       </c>
       <c r="F66">
@@ -3424,8 +3706,12 @@
       <c r="I66" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K66" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>155</v>
       </c>
@@ -3433,11 +3719,11 @@
         <v>156</v>
       </c>
       <c r="C67" s="2" t="str">
-        <f t="shared" ref="C67" si="65">IF(D67=0,"",IF(ISNUMBER(D67),TEXT(D67,"0"),D67))</f>
+        <f t="shared" ref="C67" si="66">IF(D67=0,"",IF(ISNUMBER(D67),TEXT(D67,"0"),D67))</f>
         <v/>
       </c>
       <c r="E67" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1962</v>
       </c>
       <c r="F67">
@@ -3452,8 +3738,12 @@
       <c r="I67" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K67" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>158</v>
       </c>
@@ -3461,11 +3751,11 @@
         <v>159</v>
       </c>
       <c r="C68" s="2" t="str">
-        <f t="shared" ref="C68" si="66">IF(D68=0,"",IF(ISNUMBER(D68),TEXT(D68,"0"),D68))</f>
+        <f t="shared" ref="C68" si="67">IF(D68=0,"",IF(ISNUMBER(D68),TEXT(D68,"0"),D68))</f>
         <v/>
       </c>
       <c r="E68" s="2" t="str">
-        <f t="shared" ref="C68:E79" si="67">IF(ISNUMBER(F68),TEXT(F68,"0"),F68)</f>
+        <f t="shared" ref="E68:E79" si="68">IF(ISNUMBER(F68),TEXT(F68,"0"),F68)</f>
         <v>2361</v>
       </c>
       <c r="F68">
@@ -3483,8 +3773,12 @@
       <c r="J68">
         <v>2</v>
       </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K68" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>160</v>
       </c>
@@ -3492,11 +3786,11 @@
         <v>161</v>
       </c>
       <c r="C69" s="2" t="str">
-        <f t="shared" ref="C69" si="68">IF(D69=0,"",IF(ISNUMBER(D69),TEXT(D69,"0"),D69))</f>
+        <f t="shared" ref="C69" si="69">IF(D69=0,"",IF(ISNUMBER(D69),TEXT(D69,"0"),D69))</f>
         <v/>
       </c>
       <c r="E69" s="2" t="str">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>2993</v>
       </c>
       <c r="F69">
@@ -3514,8 +3808,12 @@
       <c r="J69">
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K69" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>163</v>
       </c>
@@ -3523,11 +3821,11 @@
         <v>164</v>
       </c>
       <c r="C70" s="2" t="str">
-        <f t="shared" ref="C70" si="69">IF(D70=0,"",IF(ISNUMBER(D70),TEXT(D70,"0"),D70))</f>
+        <f t="shared" ref="C70" si="70">IF(D70=0,"",IF(ISNUMBER(D70),TEXT(D70,"0"),D70))</f>
         <v/>
       </c>
       <c r="E70" s="2" t="str">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>2590</v>
       </c>
       <c r="F70">
@@ -3545,8 +3843,12 @@
       <c r="J70">
         <v>9</v>
       </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K70" s="3" t="str">
+        <f t="shared" ref="K70:K79" si="71">K69</f>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>165</v>
       </c>
@@ -3554,11 +3856,11 @@
         <v>166</v>
       </c>
       <c r="C71" s="2" t="str">
-        <f t="shared" ref="C71" si="70">IF(D71=0,"",IF(ISNUMBER(D71),TEXT(D71,"0"),D71))</f>
+        <f t="shared" ref="C71" si="72">IF(D71=0,"",IF(ISNUMBER(D71),TEXT(D71,"0"),D71))</f>
         <v/>
       </c>
       <c r="E71" s="2" t="str">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>2475</v>
       </c>
       <c r="F71">
@@ -3576,8 +3878,12 @@
       <c r="J71">
         <v>2</v>
       </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K71" s="3" t="str">
+        <f t="shared" si="71"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>167</v>
       </c>
@@ -3585,11 +3891,11 @@
         <v>168</v>
       </c>
       <c r="C72" s="2" t="str">
-        <f t="shared" ref="C72" si="71">IF(D72=0,"",IF(ISNUMBER(D72),TEXT(D72,"0"),D72))</f>
+        <f t="shared" ref="C72" si="73">IF(D72=0,"",IF(ISNUMBER(D72),TEXT(D72,"0"),D72))</f>
         <v/>
       </c>
       <c r="E72" s="2" t="str">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>2796</v>
       </c>
       <c r="F72">
@@ -3607,8 +3913,12 @@
       <c r="J72">
         <v>6</v>
       </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K72" s="3" t="str">
+        <f t="shared" si="71"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>169</v>
       </c>
@@ -3616,14 +3926,14 @@
         <v>170</v>
       </c>
       <c r="C73" s="2" t="str">
-        <f t="shared" ref="C73" si="72">IF(D73=0,"",IF(ISNUMBER(D73),TEXT(D73,"0"),D73))</f>
+        <f t="shared" ref="C73" si="74">IF(D73=0,"",IF(ISNUMBER(D73),TEXT(D73,"0"),D73))</f>
         <v>30232101</v>
       </c>
       <c r="D73">
         <v>30232101</v>
       </c>
       <c r="E73" s="2" t="str">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>1958</v>
       </c>
       <c r="F73">
@@ -3641,8 +3951,12 @@
       <c r="J73">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K73" s="3" t="str">
+        <f t="shared" si="71"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>171</v>
       </c>
@@ -3650,11 +3964,11 @@
         <v>172</v>
       </c>
       <c r="C74" s="2" t="str">
-        <f t="shared" ref="C74" si="73">IF(D74=0,"",IF(ISNUMBER(D74),TEXT(D74,"0"),D74))</f>
+        <f t="shared" ref="C74" si="75">IF(D74=0,"",IF(ISNUMBER(D74),TEXT(D74,"0"),D74))</f>
         <v/>
       </c>
       <c r="E74" s="2" t="str">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>1963</v>
       </c>
       <c r="F74">
@@ -3672,8 +3986,12 @@
       <c r="J74">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K74" s="3" t="str">
+        <f t="shared" si="71"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>173</v>
       </c>
@@ -3681,11 +3999,11 @@
         <v>174</v>
       </c>
       <c r="C75" s="2" t="str">
-        <f t="shared" ref="C75" si="74">IF(D75=0,"",IF(ISNUMBER(D75),TEXT(D75,"0"),D75))</f>
+        <f t="shared" ref="C75" si="76">IF(D75=0,"",IF(ISNUMBER(D75),TEXT(D75,"0"),D75))</f>
         <v/>
       </c>
       <c r="E75" s="2" t="str">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>2362</v>
       </c>
       <c r="F75">
@@ -3703,8 +4021,12 @@
       <c r="J75">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K75" s="3" t="str">
+        <f t="shared" si="71"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>175</v>
       </c>
@@ -3712,11 +4034,11 @@
         <v>176</v>
       </c>
       <c r="C76" s="2" t="str">
-        <f t="shared" ref="C76" si="75">IF(D76=0,"",IF(ISNUMBER(D76),TEXT(D76,"0"),D76))</f>
+        <f t="shared" ref="C76" si="77">IF(D76=0,"",IF(ISNUMBER(D76),TEXT(D76,"0"),D76))</f>
         <v/>
       </c>
       <c r="E76" s="2" t="str">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>2364</v>
       </c>
       <c r="F76">
@@ -3734,8 +4056,12 @@
       <c r="J76">
         <v>3</v>
       </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K76" s="3" t="str">
+        <f t="shared" si="71"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>177</v>
       </c>
@@ -3743,11 +4069,11 @@
         <v>178</v>
       </c>
       <c r="C77" s="2" t="str">
-        <f t="shared" ref="C77" si="76">IF(D77=0,"",IF(ISNUMBER(D77),TEXT(D77,"0"),D77))</f>
+        <f t="shared" ref="C77" si="78">IF(D77=0,"",IF(ISNUMBER(D77),TEXT(D77,"0"),D77))</f>
         <v/>
       </c>
       <c r="E77" s="2" t="str">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>2111</v>
       </c>
       <c r="F77">
@@ -3765,8 +4091,12 @@
       <c r="J77">
         <v>1</v>
       </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K77" s="3" t="str">
+        <f t="shared" si="71"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>179</v>
       </c>
@@ -3774,11 +4104,11 @@
         <v>180</v>
       </c>
       <c r="C78" s="2" t="str">
-        <f t="shared" ref="C78" si="77">IF(D78=0,"",IF(ISNUMBER(D78),TEXT(D78,"0"),D78))</f>
+        <f t="shared" ref="C78" si="79">IF(D78=0,"",IF(ISNUMBER(D78),TEXT(D78,"0"),D78))</f>
         <v/>
       </c>
       <c r="E78" s="2" t="str">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>2470</v>
       </c>
       <c r="F78">
@@ -3796,8 +4126,12 @@
       <c r="J78">
         <v>5</v>
       </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K78" s="3" t="str">
+        <f t="shared" si="71"/>
+        <v>RDA</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>181</v>
       </c>
@@ -3805,11 +4139,11 @@
         <v>182</v>
       </c>
       <c r="C79" s="2" t="str">
-        <f t="shared" ref="C79" si="78">IF(D79=0,"",IF(ISNUMBER(D79),TEXT(D79,"0"),D79))</f>
+        <f t="shared" ref="C79" si="80">IF(D79=0,"",IF(ISNUMBER(D79),TEXT(D79,"0"),D79))</f>
         <v/>
       </c>
       <c r="E79" s="2" t="str">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>2097</v>
       </c>
       <c r="F79">
@@ -3820,6 +4154,10 @@
       </c>
       <c r="H79" t="s">
         <v>11</v>
+      </c>
+      <c r="K79" s="3" t="str">
+        <f t="shared" si="71"/>
+        <v>RDA</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MDT WIP (kostenplaatsen toegevoegd)
</commit_message>
<xml_diff>
--- a/MDT/DienstenCatalogus/Producten-RegistratieDocumentAfhandeling.xlsx
+++ b/MDT/DienstenCatalogus/Producten-RegistratieDocumentAfhandeling.xlsx
@@ -21,6 +21,41 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>hjo20125</author>
+  </authors>
+  <commentList>
+    <comment ref="A43" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>hjo20125:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Komt ook voor in VAP, maar dan met andere procID (2366)
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="194">
   <si>
@@ -336,9 +371,6 @@
     <t>G</t>
   </si>
   <si>
-    <t>OPHTAR</t>
-  </si>
-  <si>
     <t>Opheffen tarief</t>
   </si>
   <si>
@@ -573,9 +605,6 @@
     <t>PresentatieGroep</t>
   </si>
   <si>
-    <t>procId</t>
-  </si>
-  <si>
     <t>ProcID</t>
   </si>
   <si>
@@ -604,13 +633,19 @@
   </si>
   <si>
     <t>ProductVrs</t>
+  </si>
+  <si>
+    <t>procID</t>
+  </si>
+  <si>
+    <t>OPHTARxxx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -752,8 +787,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -945,6 +993,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1106,11 +1160,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1455,11 +1510,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B37" workbookViewId="0">
-      <selection activeCell="K54" sqref="K54"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1505,48 +1560,48 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C2" t="s">
+        <v>190</v>
+      </c>
+      <c r="E2" t="s">
+        <v>192</v>
+      </c>
+      <c r="H2" t="s">
+        <v>183</v>
+      </c>
+      <c r="I2" t="s">
         <v>180</v>
       </c>
-      <c r="B2" t="s">
-        <v>191</v>
-      </c>
-      <c r="C2" t="s">
-        <v>192</v>
-      </c>
-      <c r="E2" t="s">
-        <v>183</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="K2" s="3" t="s">
         <v>185</v>
-      </c>
-      <c r="I2" t="s">
-        <v>181</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E3" t="s">
+        <v>182</v>
+      </c>
+      <c r="H3" t="s">
         <v>184</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
+        <v>181</v>
+      </c>
+      <c r="K3" s="3" t="s">
         <v>186</v>
-      </c>
-      <c r="I3" t="s">
-        <v>182</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -1583,7 +1638,7 @@
         <v>3</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -2902,11 +2957,11 @@
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+      <c r="A43" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B43" t="s">
         <v>104</v>
-      </c>
-      <c r="B43" t="s">
-        <v>105</v>
       </c>
       <c r="C43" s="2" t="str">
         <f t="shared" ref="C43" si="42">IF(D43=0,"",IF(ISNUMBER(D43),TEXT(D43,"0"),D43))</f>
@@ -2926,7 +2981,7 @@
         <v>11</v>
       </c>
       <c r="I43" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K43" s="3" t="str">
         <f t="shared" si="4"/>
@@ -2935,10 +2990,10 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
+        <v>106</v>
+      </c>
+      <c r="B44" t="s">
         <v>107</v>
-      </c>
-      <c r="B44" t="s">
-        <v>108</v>
       </c>
       <c r="C44" s="2" t="str">
         <f t="shared" ref="C44" si="43">IF(D44=0,"",IF(ISNUMBER(D44),TEXT(D44,"0"),D44))</f>
@@ -2967,10 +3022,10 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>108</v>
+      </c>
+      <c r="B45" t="s">
         <v>109</v>
-      </c>
-      <c r="B45" t="s">
-        <v>110</v>
       </c>
       <c r="C45" s="2" t="str">
         <f t="shared" ref="C45" si="44">IF(D45=0,"",IF(ISNUMBER(D45),TEXT(D45,"0"),D45))</f>
@@ -3002,10 +3057,10 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>110</v>
+      </c>
+      <c r="B46" t="s">
         <v>111</v>
-      </c>
-      <c r="B46" t="s">
-        <v>112</v>
       </c>
       <c r="C46" s="2" t="str">
         <f t="shared" ref="C46" si="45">IF(D46=0,"",IF(ISNUMBER(D46),TEXT(D46,"0"),D46))</f>
@@ -3031,10 +3086,10 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
+        <v>112</v>
+      </c>
+      <c r="B47" t="s">
         <v>113</v>
-      </c>
-      <c r="B47" t="s">
-        <v>114</v>
       </c>
       <c r="C47" s="2" t="str">
         <f t="shared" ref="C47" si="46">IF(D47=0,"",IF(ISNUMBER(D47),TEXT(D47,"0"),D47))</f>
@@ -3063,10 +3118,10 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
+        <v>114</v>
+      </c>
+      <c r="B48" t="s">
         <v>115</v>
-      </c>
-      <c r="B48" t="s">
-        <v>116</v>
       </c>
       <c r="C48" s="2" t="str">
         <f t="shared" ref="C48" si="47">IF(D48=0,"",IF(ISNUMBER(D48),TEXT(D48,"0"),D48))</f>
@@ -3086,7 +3141,7 @@
         <v>11</v>
       </c>
       <c r="I48" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K48" s="3" t="str">
         <f t="shared" si="4"/>
@@ -3095,10 +3150,10 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
+        <v>117</v>
+      </c>
+      <c r="B49" t="s">
         <v>118</v>
-      </c>
-      <c r="B49" t="s">
-        <v>119</v>
       </c>
       <c r="C49" s="2" t="str">
         <f t="shared" ref="C49" si="48">IF(D49=0,"",IF(ISNUMBER(D49),TEXT(D49,"0"),D49))</f>
@@ -3118,7 +3173,7 @@
         <v>11</v>
       </c>
       <c r="I49" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J49">
         <v>1</v>
@@ -3130,10 +3185,10 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
+        <v>119</v>
+      </c>
+      <c r="B50" t="s">
         <v>120</v>
-      </c>
-      <c r="B50" t="s">
-        <v>121</v>
       </c>
       <c r="C50" s="2" t="str">
         <f t="shared" ref="C50" si="49">IF(D50=0,"",IF(ISNUMBER(D50),TEXT(D50,"0"),D50))</f>
@@ -3162,10 +3217,10 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
+        <v>121</v>
+      </c>
+      <c r="B51" t="s">
         <v>122</v>
-      </c>
-      <c r="B51" t="s">
-        <v>123</v>
       </c>
       <c r="C51" s="2" t="str">
         <f t="shared" ref="C51" si="50">IF(D51=0,"",IF(ISNUMBER(D51),TEXT(D51,"0"),D51))</f>
@@ -3194,10 +3249,10 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
+        <v>123</v>
+      </c>
+      <c r="B52" t="s">
         <v>124</v>
-      </c>
-      <c r="B52" t="s">
-        <v>125</v>
       </c>
       <c r="C52" s="2" t="str">
         <f t="shared" ref="C52" si="51">IF(D52=0,"",IF(ISNUMBER(D52),TEXT(D52,"0"),D52))</f>
@@ -3229,10 +3284,10 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
+        <v>125</v>
+      </c>
+      <c r="B53" t="s">
         <v>126</v>
-      </c>
-      <c r="B53" t="s">
-        <v>127</v>
       </c>
       <c r="C53" s="2" t="str">
         <f t="shared" ref="C53" si="52">IF(D53=0,"",IF(ISNUMBER(D53),TEXT(D53,"0"),D53))</f>
@@ -3264,10 +3319,10 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
+        <v>127</v>
+      </c>
+      <c r="B54" t="s">
         <v>128</v>
-      </c>
-      <c r="B54" t="s">
-        <v>129</v>
       </c>
       <c r="C54" s="2" t="str">
         <f t="shared" ref="C54" si="53">IF(D54=0,"",IF(ISNUMBER(D54),TEXT(D54,"0"),D54))</f>
@@ -3302,10 +3357,10 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
+        <v>129</v>
+      </c>
+      <c r="B55" t="s">
         <v>130</v>
-      </c>
-      <c r="B55" t="s">
-        <v>131</v>
       </c>
       <c r="C55" s="2" t="str">
         <f t="shared" ref="C55" si="54">IF(D55=0,"",IF(ISNUMBER(D55),TEXT(D55,"0"),D55))</f>
@@ -3337,10 +3392,10 @@
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
+        <v>131</v>
+      </c>
+      <c r="B56" t="s">
         <v>132</v>
-      </c>
-      <c r="B56" t="s">
-        <v>133</v>
       </c>
       <c r="C56" s="2" t="str">
         <f t="shared" ref="C56" si="55">IF(D56=0,"",IF(ISNUMBER(D56),TEXT(D56,"0"),D56))</f>
@@ -3372,10 +3427,10 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
+        <v>133</v>
+      </c>
+      <c r="B57" t="s">
         <v>134</v>
-      </c>
-      <c r="B57" t="s">
-        <v>135</v>
       </c>
       <c r="C57" s="2" t="str">
         <f t="shared" ref="C57" si="56">IF(D57=0,"",IF(ISNUMBER(D57),TEXT(D57,"0"),D57))</f>
@@ -3395,7 +3450,7 @@
         <v>11</v>
       </c>
       <c r="I57" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J57">
         <v>2</v>
@@ -3407,10 +3462,10 @@
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
+        <v>135</v>
+      </c>
+      <c r="B58" t="s">
         <v>136</v>
-      </c>
-      <c r="B58" t="s">
-        <v>137</v>
       </c>
       <c r="C58" s="2" t="str">
         <f t="shared" ref="C58" si="57">IF(D58=0,"",IF(ISNUMBER(D58),TEXT(D58,"0"),D58))</f>
@@ -3430,7 +3485,7 @@
         <v>11</v>
       </c>
       <c r="I58" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J58">
         <v>3</v>
@@ -3442,10 +3497,10 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
+        <v>137</v>
+      </c>
+      <c r="B59" t="s">
         <v>138</v>
-      </c>
-      <c r="B59" t="s">
-        <v>139</v>
       </c>
       <c r="C59" s="2" t="str">
         <f t="shared" ref="C59" si="58">IF(D59=0,"",IF(ISNUMBER(D59),TEXT(D59,"0"),D59))</f>
@@ -3471,10 +3526,10 @@
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
+        <v>139</v>
+      </c>
+      <c r="B60" t="s">
         <v>140</v>
-      </c>
-      <c r="B60" t="s">
-        <v>141</v>
       </c>
       <c r="C60" s="2" t="str">
         <f t="shared" ref="C60" si="59">IF(D60=0,"",IF(ISNUMBER(D60),TEXT(D60,"0"),D60))</f>
@@ -3506,10 +3561,10 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
+        <v>141</v>
+      </c>
+      <c r="B61" t="s">
         <v>142</v>
-      </c>
-      <c r="B61" t="s">
-        <v>143</v>
       </c>
       <c r="C61" s="2" t="str">
         <f t="shared" ref="C61" si="60">IF(D61=0,"",IF(ISNUMBER(D61),TEXT(D61,"0"),D61))</f>
@@ -3541,10 +3596,10 @@
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
+        <v>143</v>
+      </c>
+      <c r="B62" t="s">
         <v>144</v>
-      </c>
-      <c r="B62" t="s">
-        <v>145</v>
       </c>
       <c r="C62" s="2" t="str">
         <f t="shared" ref="C62" si="61">IF(D62=0,"",IF(ISNUMBER(D62),TEXT(D62,"0"),D62))</f>
@@ -3576,10 +3631,10 @@
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
+        <v>145</v>
+      </c>
+      <c r="B63" t="s">
         <v>146</v>
-      </c>
-      <c r="B63" t="s">
-        <v>147</v>
       </c>
       <c r="C63" s="2" t="str">
         <f t="shared" ref="C63" si="62">IF(D63=0,"",IF(ISNUMBER(D63),TEXT(D63,"0"),D63))</f>
@@ -3599,7 +3654,7 @@
         <v>11</v>
       </c>
       <c r="I63" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K63" s="3" t="str">
         <f t="shared" si="4"/>
@@ -3608,10 +3663,10 @@
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
+        <v>148</v>
+      </c>
+      <c r="B64" t="s">
         <v>149</v>
-      </c>
-      <c r="B64" t="s">
-        <v>150</v>
       </c>
       <c r="C64" s="2" t="str">
         <f t="shared" ref="C64" si="63">IF(D64=0,"",IF(ISNUMBER(D64),TEXT(D64,"0"),D64))</f>
@@ -3643,10 +3698,10 @@
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
+        <v>150</v>
+      </c>
+      <c r="B65" t="s">
         <v>151</v>
-      </c>
-      <c r="B65" t="s">
-        <v>152</v>
       </c>
       <c r="C65" s="2" t="str">
         <f t="shared" ref="C65" si="64">IF(D65=0,"",IF(ISNUMBER(D65),TEXT(D65,"0"),D65))</f>
@@ -3666,7 +3721,7 @@
         <v>11</v>
       </c>
       <c r="I65" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K65" s="3" t="str">
         <f t="shared" si="4"/>
@@ -3675,10 +3730,10 @@
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
+        <v>153</v>
+      </c>
+      <c r="B66" t="s">
         <v>154</v>
-      </c>
-      <c r="B66" t="s">
-        <v>155</v>
       </c>
       <c r="C66" s="2" t="str">
         <f t="shared" ref="C66" si="65">IF(D66=0,"",IF(ISNUMBER(D66),TEXT(D66,"0"),D66))</f>
@@ -3710,10 +3765,10 @@
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
+        <v>155</v>
+      </c>
+      <c r="B67" t="s">
         <v>156</v>
-      </c>
-      <c r="B67" t="s">
-        <v>157</v>
       </c>
       <c r="C67" s="2" t="str">
         <f t="shared" ref="C67" si="67">IF(D67=0,"",IF(ISNUMBER(D67),TEXT(D67,"0"),D67))</f>
@@ -3733,7 +3788,7 @@
         <v>11</v>
       </c>
       <c r="I67" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J67">
         <v>1</v>
@@ -3745,10 +3800,10 @@
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
+        <v>158</v>
+      </c>
+      <c r="B68" t="s">
         <v>159</v>
-      </c>
-      <c r="B68" t="s">
-        <v>160</v>
       </c>
       <c r="C68" s="2" t="str">
         <f t="shared" ref="C68" si="68">IF(D68=0,"",IF(ISNUMBER(D68),TEXT(D68,"0"),D68))</f>
@@ -3780,10 +3835,10 @@
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
+        <v>160</v>
+      </c>
+      <c r="B69" t="s">
         <v>161</v>
-      </c>
-      <c r="B69" t="s">
-        <v>162</v>
       </c>
       <c r="C69" s="2" t="str">
         <f t="shared" ref="C69" si="70">IF(D69=0,"",IF(ISNUMBER(D69),TEXT(D69,"0"),D69))</f>
@@ -3815,10 +3870,10 @@
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
+        <v>162</v>
+      </c>
+      <c r="B70" t="s">
         <v>163</v>
-      </c>
-      <c r="B70" t="s">
-        <v>164</v>
       </c>
       <c r="C70" s="2" t="str">
         <f t="shared" ref="C70" si="71">IF(D70=0,"",IF(ISNUMBER(D70),TEXT(D70,"0"),D70))</f>
@@ -3850,10 +3905,10 @@
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
+        <v>164</v>
+      </c>
+      <c r="B71" t="s">
         <v>165</v>
-      </c>
-      <c r="B71" t="s">
-        <v>166</v>
       </c>
       <c r="C71" s="2" t="str">
         <f t="shared" ref="C71" si="72">IF(D71=0,"",IF(ISNUMBER(D71),TEXT(D71,"0"),D71))</f>
@@ -3888,10 +3943,10 @@
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
+        <v>166</v>
+      </c>
+      <c r="B72" t="s">
         <v>167</v>
-      </c>
-      <c r="B72" t="s">
-        <v>168</v>
       </c>
       <c r="C72" s="2" t="str">
         <f t="shared" ref="C72" si="73">IF(D72=0,"",IF(ISNUMBER(D72),TEXT(D72,"0"),D72))</f>
@@ -3911,7 +3966,7 @@
         <v>11</v>
       </c>
       <c r="I72" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J72">
         <v>1</v>
@@ -3923,10 +3978,10 @@
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
+        <v>168</v>
+      </c>
+      <c r="B73" t="s">
         <v>169</v>
-      </c>
-      <c r="B73" t="s">
-        <v>170</v>
       </c>
       <c r="C73" s="2" t="str">
         <f t="shared" ref="C73" si="74">IF(D73=0,"",IF(ISNUMBER(D73),TEXT(D73,"0"),D73))</f>
@@ -3958,10 +4013,10 @@
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
+        <v>170</v>
+      </c>
+      <c r="B74" t="s">
         <v>171</v>
-      </c>
-      <c r="B74" t="s">
-        <v>172</v>
       </c>
       <c r="C74" s="2" t="str">
         <f t="shared" ref="C74" si="75">IF(D74=0,"",IF(ISNUMBER(D74),TEXT(D74,"0"),D74))</f>
@@ -3993,10 +4048,10 @@
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
+        <v>172</v>
+      </c>
+      <c r="B75" t="s">
         <v>173</v>
-      </c>
-      <c r="B75" t="s">
-        <v>174</v>
       </c>
       <c r="C75" s="2" t="str">
         <f t="shared" ref="C75" si="76">IF(D75=0,"",IF(ISNUMBER(D75),TEXT(D75,"0"),D75))</f>
@@ -4028,10 +4083,10 @@
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
+        <v>174</v>
+      </c>
+      <c r="B76" t="s">
         <v>175</v>
-      </c>
-      <c r="B76" t="s">
-        <v>176</v>
       </c>
       <c r="C76" s="2" t="str">
         <f t="shared" ref="C76" si="77">IF(D76=0,"",IF(ISNUMBER(D76),TEXT(D76,"0"),D76))</f>
@@ -4063,10 +4118,10 @@
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
+        <v>176</v>
+      </c>
+      <c r="B77" t="s">
         <v>177</v>
-      </c>
-      <c r="B77" t="s">
-        <v>178</v>
       </c>
       <c r="C77" s="2" t="str">
         <f t="shared" ref="C77" si="78">IF(D77=0,"",IF(ISNUMBER(D77),TEXT(D77,"0"),D77))</f>
@@ -4093,5 +4148,6 @@
   </sheetData>
   <autoFilter ref="A1:J77"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>